<commit_message>
Finalized and cleaned config code for Env Rep team
</commit_message>
<xml_diff>
--- a/utils/config/ReferenceLists/consolidatedUnits.xlsx
+++ b/utils/config/ReferenceLists/consolidatedUnits.xlsx
@@ -674,7 +674,7 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>109</v>
+        <v>218</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -1044,7 +1044,7 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>132993</v>
+        <v>1063944</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1110,7 +1110,7 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>132993</v>
+        <v>1063944</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1747,7 +1747,7 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>352140</v>
+        <v>1056420</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1900,7 +1900,7 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>1164</v>
+        <v>2328</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -1979,7 +1979,7 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>6200</v>
+        <v>18600</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -2190,7 +2190,7 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>6200</v>
+        <v>18600</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -3382,7 +3382,7 @@
         </is>
       </c>
       <c r="G45" t="n">
-        <v>55369</v>
+        <v>110738</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
@@ -3535,7 +3535,7 @@
         </is>
       </c>
       <c r="G47" t="n">
-        <v>54421</v>
+        <v>163263</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
@@ -3772,7 +3772,7 @@
         </is>
       </c>
       <c r="G50" t="n">
-        <v>54421</v>
+        <v>163263</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
@@ -3846,7 +3846,7 @@
         </is>
       </c>
       <c r="G51" t="n">
-        <v>55369</v>
+        <v>110738</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
@@ -4996,7 +4996,7 @@
         </is>
       </c>
       <c r="G66" t="n">
-        <v>352140</v>
+        <v>1056420</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
@@ -5075,7 +5075,7 @@
         </is>
       </c>
       <c r="G67" t="n">
-        <v>352140</v>
+        <v>1056420</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
@@ -5763,7 +5763,7 @@
         </is>
       </c>
       <c r="G76" t="n">
-        <v>132993</v>
+        <v>1063944</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
@@ -7431,7 +7431,7 @@
         </is>
       </c>
       <c r="G99" t="n">
-        <v>54421</v>
+        <v>163263</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
@@ -7510,7 +7510,7 @@
         </is>
       </c>
       <c r="G100" t="n">
-        <v>843</v>
+        <v>1686</v>
       </c>
       <c r="H100" t="inlineStr">
         <is>
@@ -7790,7 +7790,7 @@
         </is>
       </c>
       <c r="G104" t="n">
-        <v>132993</v>
+        <v>1063944</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
@@ -7856,7 +7856,7 @@
         </is>
       </c>
       <c r="G105" t="n">
-        <v>1164</v>
+        <v>2328</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
@@ -8376,7 +8376,7 @@
         </is>
       </c>
       <c r="G113" t="n">
-        <v>132993</v>
+        <v>1063944</v>
       </c>
       <c r="H113" t="inlineStr">
         <is>
@@ -8442,7 +8442,7 @@
         </is>
       </c>
       <c r="G114" t="n">
-        <v>843</v>
+        <v>1686</v>
       </c>
       <c r="H114" t="inlineStr">
         <is>
@@ -8643,7 +8643,7 @@
         </is>
       </c>
       <c r="G117" t="n">
-        <v>132993</v>
+        <v>1063944</v>
       </c>
       <c r="H117" t="inlineStr">
         <is>
@@ -8709,7 +8709,7 @@
         </is>
       </c>
       <c r="G118" t="n">
-        <v>132993</v>
+        <v>1063944</v>
       </c>
       <c r="H118" t="inlineStr">
         <is>
@@ -8841,7 +8841,7 @@
         </is>
       </c>
       <c r="G120" t="n">
-        <v>132993</v>
+        <v>1063944</v>
       </c>
       <c r="H120" t="inlineStr">
         <is>
@@ -9039,7 +9039,7 @@
         </is>
       </c>
       <c r="G123" t="n">
-        <v>6200</v>
+        <v>18600</v>
       </c>
       <c r="H123" t="inlineStr">
         <is>
@@ -9278,7 +9278,7 @@
         </is>
       </c>
       <c r="G127" t="n">
-        <v>109</v>
+        <v>218</v>
       </c>
       <c r="I127" t="n">
         <v>0</v>

</xml_diff>